<commit_message>
Changes for PSG and Platform up to 5/21/2018
</commit_message>
<xml_diff>
--- a/doc/messagesDefinition-v1.xlsx
+++ b/doc/messagesDefinition-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_wk\builds\dds-launchpad-iiot-poc-psg-pub\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_wk\_p\dds-launchpad-iiot-poc-psg-pub\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE28A7AF-EBD5-4B93-BEEE-772AB856036E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151F9272-230D-463C-9898-2E46BEF61504}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21317" windowHeight="12394" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21317" windowHeight="12394" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="messageSchema" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
   <si>
     <t>timestamp</t>
   </si>
@@ -38,9 +38,6 @@
     <t>magnitude</t>
   </si>
   <si>
-    <t>temperature</t>
-  </si>
-  <si>
     <t>batteryLevel</t>
   </si>
   <si>
@@ -189,6 +186,12 @@
   </si>
   <si>
     <t>sensorIndex</t>
+  </si>
+  <si>
+    <t>tempExternal</t>
+  </si>
+  <si>
+    <t>tempInternal</t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -560,123 +563,132 @@
     <col min="4" max="4" width="14.3046875" customWidth="1"/>
     <col min="5" max="5" width="20.15234375" customWidth="1"/>
     <col min="6" max="6" width="13.53515625" customWidth="1"/>
-    <col min="7" max="7" width="12.53515625" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="16.53515625" customWidth="1"/>
-    <col min="10" max="10" width="30" customWidth="1"/>
-    <col min="11" max="11" width="26.84375" customWidth="1"/>
+    <col min="7" max="8" width="12.53515625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="16.53515625" customWidth="1"/>
+    <col min="11" max="11" width="30" customWidth="1"/>
+    <col min="12" max="12" width="26.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>-255</v>
+      </c>
+      <c r="H4">
+        <v>-255</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>11</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>12</v>
       </c>
       <c r="F5">
         <v>7</v>
@@ -688,75 +700,84 @@
         <v>4096</v>
       </c>
       <c r="I5">
+        <v>4096</v>
+      </c>
+      <c r="J5">
         <v>1000</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>255</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>-50</v>
+      </c>
+      <c r="H6">
+        <v>-50</v>
+      </c>
+      <c r="I6">
+        <v>2700</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="G6">
-        <v>233</v>
-      </c>
-      <c r="H6">
-        <v>2700</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
       <c r="G7">
-        <v>358</v>
+        <v>200</v>
       </c>
       <c r="H7">
+        <v>200</v>
+      </c>
+      <c r="I7">
         <v>3600</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>255</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K16" s="1"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -765,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -778,123 +799,132 @@
     <col min="4" max="4" width="14.3046875" customWidth="1"/>
     <col min="5" max="5" width="20.15234375" customWidth="1"/>
     <col min="6" max="6" width="13.53515625" customWidth="1"/>
-    <col min="7" max="7" width="12.53515625" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="16.53515625" customWidth="1"/>
-    <col min="10" max="10" width="255.69140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="182.53515625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="12.53515625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="16.53515625" customWidth="1"/>
+    <col min="11" max="11" width="255.69140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="182.53515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>-255</v>
+      </c>
+      <c r="H4">
+        <v>-255</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>11</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>12</v>
       </c>
       <c r="F5">
         <v>7</v>
@@ -906,340 +936,376 @@
         <v>4096</v>
       </c>
       <c r="I5">
+        <v>4096</v>
+      </c>
+      <c r="J5">
         <v>1000</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>255</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>-50</v>
+      </c>
+      <c r="H6">
+        <v>-50</v>
+      </c>
+      <c r="I6">
+        <v>2700</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="G6">
-        <v>233</v>
-      </c>
-      <c r="H6">
-        <v>2700</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
       <c r="G7">
-        <v>358</v>
+        <v>200</v>
       </c>
       <c r="H7">
+        <v>200</v>
+      </c>
+      <c r="I7">
         <v>3600</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>255</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>250</v>
+        <v>65</v>
       </c>
       <c r="H8">
+        <v>75</v>
+      </c>
+      <c r="I8">
         <v>3000</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>100</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>10000</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="H9">
+        <v>70</v>
+      </c>
+      <c r="I9">
         <v>2500</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>100</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>20000</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="H10">
+        <v>130</v>
+      </c>
+      <c r="I10">
         <v>3500</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>100</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>5000</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="I11">
         <v>3001</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>100</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10000</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>4</v>
       </c>
       <c r="G12">
-        <v>176</v>
+        <v>32</v>
       </c>
       <c r="H12">
+        <v>38</v>
+      </c>
+      <c r="I12">
         <v>2501</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>100</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>20000</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13">
         <v>5</v>
       </c>
       <c r="G13">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
         <v>3501</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>100</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>15000</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14">
         <v>6</v>
       </c>
       <c r="G14">
-        <v>235</v>
+        <v>-20</v>
       </c>
       <c r="H14">
+        <v>-16</v>
+      </c>
+      <c r="I14">
         <v>3002</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>100</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>10000</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15">
         <v>7</v>
       </c>
       <c r="G15">
-        <v>202</v>
+        <v>-30</v>
       </c>
       <c r="H15">
+        <v>-20</v>
+      </c>
+      <c r="I15">
         <v>2502</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>100</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>20000</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>165</v>
+        <v>-49</v>
       </c>
       <c r="H16">
+        <v>-40</v>
+      </c>
+      <c r="I16">
         <v>3503</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>100</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>52</v>
+      <c r="K16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1250,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8977B2-AAE5-4B3C-96B4-E86BDEB69204}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1264,170 +1330,182 @@
     <col min="4" max="4" width="7.765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.3828125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.4609375" customWidth="1"/>
-    <col min="7" max="7" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.61328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="36.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.61328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="36.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
       <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="H2">
+        <v>105</v>
+      </c>
+      <c r="I2">
         <v>3000</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>10000</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
       <c r="G3">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
         <v>2500</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>10000</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
       <c r="G4">
-        <v>180</v>
+        <v>-20</v>
       </c>
       <c r="H4">
+        <v>-10</v>
+      </c>
+      <c r="I4">
         <v>3500</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>10</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J5" s="2"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J6" s="2"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="J11" s="2"/>
+      <c r="L4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K9" s="2"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>